<commit_message>
imputations donegit add .!  woohoo!
</commit_message>
<xml_diff>
--- a/04_scratch_work/01_notes/imputation_plan.xlsx
+++ b/04_scratch_work/01_notes/imputation_plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Git_Stuff\General_Assembly\04_Projects\project-capstone\dsb318-capstone\04_scratch_work\01_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E40CA5-B7E5-4DF4-AAD3-E17932018387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9983D4-ECE4-42CC-AF0E-940333BE1B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4EBB2F9C-10F1-4AA4-837D-8712C424BD66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="255">
   <si>
     <t>w1q64_12</t>
   </si>
@@ -796,6 +797,9 @@
   </si>
   <si>
     <t>So I need to figure out how to fix them, then re-run the simple imputer.</t>
+  </si>
+  <si>
+    <t>left out earlier</t>
   </si>
 </sst>
 </file>
@@ -1170,15 +1174,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8288AE37-69F5-42DE-A155-23650471245B}">
   <dimension ref="A1:D227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F185" sqref="F185"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1251,7 +1255,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1262,7 +1266,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1273,7 +1277,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1284,7 +1288,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1295,7 +1299,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1310,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1317,7 +1321,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1328,7 +1332,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1361,7 +1365,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1372,7 +1376,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1383,7 +1387,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1394,7 +1398,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1405,7 +1409,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -1416,7 +1420,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -1427,7 +1431,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>156</v>
       </c>
@@ -1438,8 +1442,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -1538,7 +1541,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1648,7 +1651,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1692,7 +1695,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>75</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -1769,7 +1772,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>80</v>
       </c>
@@ -1780,7 +1783,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>81</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>82</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>83</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>84</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>91</v>
       </c>
@@ -1879,7 +1882,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>92</v>
       </c>
@@ -1890,7 +1893,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>93</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>94</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>96</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>97</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>98</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>99</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>100</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>101</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>104</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>105</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>106</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>108</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>111</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>112</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -2165,7 +2168,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -2176,7 +2179,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>15</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>18</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>22</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>23</v>
       </c>
@@ -2308,7 +2311,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>27</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>28</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>29</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>31</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>33</v>
       </c>
@@ -2385,7 +2388,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>37</v>
       </c>
@@ -2396,7 +2399,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>38</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>39</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -2429,7 +2432,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>46</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>55</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>56</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>62</v>
       </c>
@@ -2473,7 +2476,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>77</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>88</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>89</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>14</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>157</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>152</v>
       </c>
@@ -2550,7 +2553,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>169</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>131</v>
       </c>
@@ -3173,7 +3176,7 @@
       </c>
       <c r="D187" s="1"/>
     </row>
-    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>172</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>173</v>
       </c>
@@ -3195,7 +3198,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>179</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>184</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>183</v>
       </c>
@@ -3228,7 +3231,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>182</v>
       </c>
@@ -3239,7 +3242,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>181</v>
       </c>
@@ -3250,7 +3253,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>180</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>187</v>
       </c>
@@ -3272,7 +3275,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>189</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>186</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>188</v>
       </c>
@@ -3305,7 +3308,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>185</v>
       </c>
@@ -3316,7 +3319,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>192</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>190</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>191</v>
       </c>
@@ -3349,7 +3352,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>193</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>194</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>195</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>196</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>197</v>
       </c>
@@ -3404,7 +3407,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="211" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>198</v>
       </c>
@@ -3415,7 +3418,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>199</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>201</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="214" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>202</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>200</v>
       </c>
@@ -3459,7 +3462,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="216" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>203</v>
       </c>
@@ -3470,7 +3473,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>204</v>
       </c>
@@ -3481,7 +3484,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>205</v>
       </c>
@@ -3492,7 +3495,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>206</v>
       </c>
@@ -3503,7 +3506,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>209</v>
       </c>
@@ -3514,7 +3517,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="221" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>208</v>
       </c>
@@ -3525,7 +3528,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="222" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>207</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="223" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>210</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>211</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>214</v>
       </c>
@@ -3569,7 +3572,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>213</v>
       </c>
@@ -3580,7 +3583,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="227" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>212</v>
       </c>
@@ -3597,4 +3600,2616 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008A8FD0-F23E-485F-8052-1D1CA781E53B}">
+  <dimension ref="A1:D218"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="2">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>227</v>
+      </c>
+      <c r="D14" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>227</v>
+      </c>
+      <c r="D28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>233</v>
+      </c>
+      <c r="D31" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>233</v>
+      </c>
+      <c r="D33" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>233</v>
+      </c>
+      <c r="D35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>233</v>
+      </c>
+      <c r="D36" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>231</v>
+      </c>
+      <c r="D37" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>248</v>
+      </c>
+      <c r="D38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>226</v>
+      </c>
+      <c r="D39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="1">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="1">
+        <v>17</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B43" s="1">
+        <v>18</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="1">
+        <v>24</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>1469</v>
+      </c>
+      <c r="C45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46">
+        <v>1356</v>
+      </c>
+      <c r="C46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47">
+        <v>1139</v>
+      </c>
+      <c r="C47" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48">
+        <v>974</v>
+      </c>
+      <c r="C48" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>1445</v>
+      </c>
+      <c r="C49" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50">
+        <v>1378</v>
+      </c>
+      <c r="C50" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51">
+        <v>1365</v>
+      </c>
+      <c r="C51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52">
+        <v>1359</v>
+      </c>
+      <c r="C52" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53">
+        <v>1391</v>
+      </c>
+      <c r="C53" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54">
+        <v>1429</v>
+      </c>
+      <c r="C54" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55">
+        <v>1451</v>
+      </c>
+      <c r="C55" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56">
+        <v>1290</v>
+      </c>
+      <c r="C56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57">
+        <v>1297</v>
+      </c>
+      <c r="C57" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58">
+        <v>1444</v>
+      </c>
+      <c r="C58" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60">
+        <v>63</v>
+      </c>
+      <c r="C60" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62">
+        <v>1065</v>
+      </c>
+      <c r="C62" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63">
+        <v>1214</v>
+      </c>
+      <c r="C63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B64">
+        <v>873</v>
+      </c>
+      <c r="C64" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65">
+        <v>1262</v>
+      </c>
+      <c r="C65" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>1076</v>
+      </c>
+      <c r="C66" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>1097</v>
+      </c>
+      <c r="C67" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68">
+        <v>1136</v>
+      </c>
+      <c r="C68" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69">
+        <v>757</v>
+      </c>
+      <c r="C69" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70">
+        <v>932</v>
+      </c>
+      <c r="C70" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71">
+        <v>1203</v>
+      </c>
+      <c r="C71" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72">
+        <v>621</v>
+      </c>
+      <c r="C72" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>93</v>
+      </c>
+      <c r="B73">
+        <v>695</v>
+      </c>
+      <c r="C73" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74">
+        <v>627</v>
+      </c>
+      <c r="C74" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>90</v>
+      </c>
+      <c r="B75">
+        <v>760</v>
+      </c>
+      <c r="C75" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76">
+        <v>691</v>
+      </c>
+      <c r="C76" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77">
+        <v>694</v>
+      </c>
+      <c r="C77" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78">
+        <v>667</v>
+      </c>
+      <c r="C78" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>100</v>
+      </c>
+      <c r="B79">
+        <v>589</v>
+      </c>
+      <c r="C79" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80">
+        <v>669</v>
+      </c>
+      <c r="C80" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81">
+        <v>738</v>
+      </c>
+      <c r="C81" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82">
+        <v>117</v>
+      </c>
+      <c r="C82" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>105</v>
+      </c>
+      <c r="B83">
+        <v>121</v>
+      </c>
+      <c r="C83" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84">
+        <v>116</v>
+      </c>
+      <c r="C84" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>104</v>
+      </c>
+      <c r="B85">
+        <v>123</v>
+      </c>
+      <c r="C85" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>107</v>
+      </c>
+      <c r="B86">
+        <v>119</v>
+      </c>
+      <c r="C86" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87">
+        <v>118</v>
+      </c>
+      <c r="C87" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88">
+        <v>110</v>
+      </c>
+      <c r="C88" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89">
+        <v>114</v>
+      </c>
+      <c r="C89" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90">
+        <v>121</v>
+      </c>
+      <c r="C90" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91">
+        <v>123</v>
+      </c>
+      <c r="C91" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>74</v>
+      </c>
+      <c r="B92">
+        <v>1024</v>
+      </c>
+      <c r="C92" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93">
+        <v>1135</v>
+      </c>
+      <c r="C93" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94">
+        <v>1033</v>
+      </c>
+      <c r="C94" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>48</v>
+      </c>
+      <c r="B95">
+        <v>1216</v>
+      </c>
+      <c r="C95" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>57</v>
+      </c>
+      <c r="B96">
+        <v>1154</v>
+      </c>
+      <c r="C96" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>61</v>
+      </c>
+      <c r="B97">
+        <v>1126</v>
+      </c>
+      <c r="C97" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98">
+        <v>1011</v>
+      </c>
+      <c r="C98" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>71</v>
+      </c>
+      <c r="B99">
+        <v>1042</v>
+      </c>
+      <c r="C99" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100">
+        <v>1096</v>
+      </c>
+      <c r="C100" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101">
+        <v>1182</v>
+      </c>
+      <c r="C101" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>83</v>
+      </c>
+      <c r="B102">
+        <v>915</v>
+      </c>
+      <c r="C102" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>50</v>
+      </c>
+      <c r="B103">
+        <v>1208</v>
+      </c>
+      <c r="C103" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>87</v>
+      </c>
+      <c r="B104">
+        <v>847</v>
+      </c>
+      <c r="C104" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>41</v>
+      </c>
+      <c r="B105">
+        <v>1300</v>
+      </c>
+      <c r="C105" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>63</v>
+      </c>
+      <c r="B106">
+        <v>1100</v>
+      </c>
+      <c r="C106" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>75</v>
+      </c>
+      <c r="B107">
+        <v>1017</v>
+      </c>
+      <c r="C107" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>69</v>
+      </c>
+      <c r="B108">
+        <v>1066</v>
+      </c>
+      <c r="C108" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>84</v>
+      </c>
+      <c r="B109">
+        <v>886</v>
+      </c>
+      <c r="C109" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>82</v>
+      </c>
+      <c r="B110">
+        <v>929</v>
+      </c>
+      <c r="C110" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>47</v>
+      </c>
+      <c r="B111">
+        <v>1230</v>
+      </c>
+      <c r="C111" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>72</v>
+      </c>
+      <c r="B112">
+        <v>1038</v>
+      </c>
+      <c r="C112" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>51</v>
+      </c>
+      <c r="B113">
+        <v>1204</v>
+      </c>
+      <c r="C113" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114">
+        <v>972</v>
+      </c>
+      <c r="C114" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>44</v>
+      </c>
+      <c r="B115">
+        <v>1269</v>
+      </c>
+      <c r="C115" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>80</v>
+      </c>
+      <c r="B116">
+        <v>965</v>
+      </c>
+      <c r="C116" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>66</v>
+      </c>
+      <c r="B117">
+        <v>1093</v>
+      </c>
+      <c r="C117" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>68</v>
+      </c>
+      <c r="B118">
+        <v>1077</v>
+      </c>
+      <c r="C118" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>85</v>
+      </c>
+      <c r="B119">
+        <v>876</v>
+      </c>
+      <c r="C119" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>101</v>
+      </c>
+      <c r="B120">
+        <v>520</v>
+      </c>
+      <c r="C120" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>53</v>
+      </c>
+      <c r="B121">
+        <v>1197</v>
+      </c>
+      <c r="C121" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>89</v>
+      </c>
+      <c r="B122">
+        <v>809</v>
+      </c>
+      <c r="C122" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>46</v>
+      </c>
+      <c r="B123">
+        <v>1235</v>
+      </c>
+      <c r="C123" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>38</v>
+      </c>
+      <c r="B124">
+        <v>1331</v>
+      </c>
+      <c r="C124" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>18</v>
+      </c>
+      <c r="B125">
+        <v>1452</v>
+      </c>
+      <c r="C125" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>28</v>
+      </c>
+      <c r="B126">
+        <v>1419</v>
+      </c>
+      <c r="C126" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>17</v>
+      </c>
+      <c r="B127">
+        <v>1454</v>
+      </c>
+      <c r="C127" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>55</v>
+      </c>
+      <c r="B128">
+        <v>1179</v>
+      </c>
+      <c r="C128" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B129">
+        <v>1464</v>
+      </c>
+      <c r="C129" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>33</v>
+      </c>
+      <c r="B130">
+        <v>1375</v>
+      </c>
+      <c r="C130" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>88</v>
+      </c>
+      <c r="B131">
+        <v>839</v>
+      </c>
+      <c r="C131" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>102</v>
+      </c>
+      <c r="B132">
+        <v>505</v>
+      </c>
+      <c r="C132" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133">
+        <v>1463</v>
+      </c>
+      <c r="C133" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>16</v>
+      </c>
+      <c r="B134">
+        <v>1458</v>
+      </c>
+      <c r="C134" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>37</v>
+      </c>
+      <c r="B135">
+        <v>1352</v>
+      </c>
+      <c r="C135" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>31</v>
+      </c>
+      <c r="B136">
+        <v>1388</v>
+      </c>
+      <c r="C136" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137">
+        <v>1483</v>
+      </c>
+      <c r="C137" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>5</v>
+      </c>
+      <c r="B138">
+        <v>1487</v>
+      </c>
+      <c r="C138" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139">
+        <v>1507</v>
+      </c>
+      <c r="C139" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>13</v>
+      </c>
+      <c r="B140">
+        <v>1464</v>
+      </c>
+      <c r="C140" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>77</v>
+      </c>
+      <c r="B141">
+        <v>972</v>
+      </c>
+      <c r="C141" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>29</v>
+      </c>
+      <c r="B142">
+        <v>1406</v>
+      </c>
+      <c r="C142" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>62</v>
+      </c>
+      <c r="B143">
+        <v>1123</v>
+      </c>
+      <c r="C143" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>1496</v>
+      </c>
+      <c r="C144" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>27</v>
+      </c>
+      <c r="B145">
+        <v>1418</v>
+      </c>
+      <c r="C145" t="s">
+        <v>239</v>
+      </c>
+      <c r="D145"/>
+    </row>
+    <row r="146" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>15</v>
+      </c>
+      <c r="B146">
+        <v>1460</v>
+      </c>
+      <c r="C146" t="s">
+        <v>239</v>
+      </c>
+      <c r="D146"/>
+    </row>
+    <row r="147" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>22</v>
+      </c>
+      <c r="B147">
+        <v>1436</v>
+      </c>
+      <c r="C147" t="s">
+        <v>239</v>
+      </c>
+      <c r="D147"/>
+    </row>
+    <row r="148" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>40</v>
+      </c>
+      <c r="B148">
+        <v>1318</v>
+      </c>
+      <c r="C148" t="s">
+        <v>239</v>
+      </c>
+      <c r="D148"/>
+    </row>
+    <row r="149" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>23</v>
+      </c>
+      <c r="B149">
+        <v>1432</v>
+      </c>
+      <c r="C149" t="s">
+        <v>239</v>
+      </c>
+      <c r="D149"/>
+    </row>
+    <row r="150" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>26</v>
+      </c>
+      <c r="B150">
+        <v>1422</v>
+      </c>
+      <c r="C150" t="s">
+        <v>239</v>
+      </c>
+      <c r="D150"/>
+    </row>
+    <row r="151" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151">
+        <v>1476</v>
+      </c>
+      <c r="C151" t="s">
+        <v>239</v>
+      </c>
+      <c r="D151"/>
+    </row>
+    <row r="152" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>9</v>
+      </c>
+      <c r="B152">
+        <v>1473</v>
+      </c>
+      <c r="C152" t="s">
+        <v>239</v>
+      </c>
+      <c r="D152"/>
+    </row>
+    <row r="153" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B153">
+        <v>1480</v>
+      </c>
+      <c r="C153" t="s">
+        <v>239</v>
+      </c>
+      <c r="D153"/>
+    </row>
+    <row r="154" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>4</v>
+      </c>
+      <c r="B154">
+        <v>1488</v>
+      </c>
+      <c r="C154" t="s">
+        <v>239</v>
+      </c>
+      <c r="D154"/>
+    </row>
+    <row r="155" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>24</v>
+      </c>
+      <c r="B155">
+        <v>1430</v>
+      </c>
+      <c r="C155" t="s">
+        <v>239</v>
+      </c>
+      <c r="D155"/>
+    </row>
+    <row r="156" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>39</v>
+      </c>
+      <c r="B156">
+        <v>1322</v>
+      </c>
+      <c r="C156" t="s">
+        <v>239</v>
+      </c>
+      <c r="D156"/>
+    </row>
+    <row r="157" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>56</v>
+      </c>
+      <c r="B157">
+        <v>1168</v>
+      </c>
+      <c r="C157" t="s">
+        <v>239</v>
+      </c>
+      <c r="D157"/>
+    </row>
+    <row r="158" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>3</v>
+      </c>
+      <c r="B158">
+        <v>1493</v>
+      </c>
+      <c r="C158" t="s">
+        <v>239</v>
+      </c>
+      <c r="D158"/>
+    </row>
+    <row r="159" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159">
+        <v>1494</v>
+      </c>
+      <c r="C159" t="s">
+        <v>239</v>
+      </c>
+      <c r="D159"/>
+    </row>
+    <row r="160" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>14</v>
+      </c>
+      <c r="B160">
+        <v>1462</v>
+      </c>
+      <c r="C160" t="s">
+        <v>246</v>
+      </c>
+      <c r="D160"/>
+    </row>
+    <row r="161" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>157</v>
+      </c>
+      <c r="B161">
+        <v>18</v>
+      </c>
+      <c r="C161" t="s">
+        <v>218</v>
+      </c>
+      <c r="D161"/>
+    </row>
+    <row r="162" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>169</v>
+      </c>
+      <c r="B162">
+        <v>17</v>
+      </c>
+      <c r="C162" t="s">
+        <v>230</v>
+      </c>
+      <c r="D162"/>
+    </row>
+    <row r="163" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>152</v>
+      </c>
+      <c r="B163">
+        <v>19</v>
+      </c>
+      <c r="C163" t="s">
+        <v>230</v>
+      </c>
+      <c r="D163"/>
+    </row>
+    <row r="164" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>131</v>
+      </c>
+      <c r="B164">
+        <v>24</v>
+      </c>
+      <c r="C164" t="s">
+        <v>240</v>
+      </c>
+      <c r="D164"/>
+    </row>
+    <row r="165" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>120</v>
+      </c>
+      <c r="B165">
+        <v>31</v>
+      </c>
+      <c r="C165" t="s">
+        <v>227</v>
+      </c>
+      <c r="D165"/>
+    </row>
+    <row r="166" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>153</v>
+      </c>
+      <c r="B166">
+        <v>19</v>
+      </c>
+      <c r="C166" t="s">
+        <v>227</v>
+      </c>
+      <c r="D166"/>
+    </row>
+    <row r="167" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>174</v>
+      </c>
+      <c r="B167">
+        <v>17</v>
+      </c>
+      <c r="C167" t="s">
+        <v>227</v>
+      </c>
+      <c r="D167"/>
+    </row>
+    <row r="168" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>18</v>
+      </c>
+      <c r="C168" t="s">
+        <v>227</v>
+      </c>
+      <c r="D168"/>
+    </row>
+    <row r="169" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>166</v>
+      </c>
+      <c r="B169">
+        <v>18</v>
+      </c>
+      <c r="C169" t="s">
+        <v>227</v>
+      </c>
+      <c r="D169"/>
+    </row>
+    <row r="170" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>149</v>
+      </c>
+      <c r="B170">
+        <v>19</v>
+      </c>
+      <c r="C170" t="s">
+        <v>227</v>
+      </c>
+      <c r="D170"/>
+    </row>
+    <row r="171" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>151</v>
+      </c>
+      <c r="B171">
+        <v>19</v>
+      </c>
+      <c r="C171" t="s">
+        <v>227</v>
+      </c>
+      <c r="D171"/>
+    </row>
+    <row r="172" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>144</v>
+      </c>
+      <c r="B172">
+        <v>18</v>
+      </c>
+      <c r="C172" t="s">
+        <v>227</v>
+      </c>
+      <c r="D172"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>137</v>
+      </c>
+      <c r="B173">
+        <v>19</v>
+      </c>
+      <c r="C173" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>124</v>
+      </c>
+      <c r="B174">
+        <v>26</v>
+      </c>
+      <c r="C174" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>118</v>
+      </c>
+      <c r="B175">
+        <v>34</v>
+      </c>
+      <c r="C175" t="s">
+        <v>227</v>
+      </c>
+      <c r="D175"/>
+    </row>
+    <row r="176" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>122</v>
+      </c>
+      <c r="B176">
+        <v>28</v>
+      </c>
+      <c r="C176" t="s">
+        <v>227</v>
+      </c>
+      <c r="D176"/>
+    </row>
+    <row r="177" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>117</v>
+      </c>
+      <c r="B177">
+        <v>38</v>
+      </c>
+      <c r="C177" t="s">
+        <v>227</v>
+      </c>
+      <c r="D177"/>
+    </row>
+    <row r="178" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>119</v>
+      </c>
+      <c r="B178">
+        <v>31</v>
+      </c>
+      <c r="C178" t="s">
+        <v>227</v>
+      </c>
+      <c r="D178"/>
+    </row>
+    <row r="179" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B179" s="2">
+        <v>18</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B180" s="2">
+        <v>18</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B181" s="2">
+        <v>20</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B182" s="2">
+        <v>18</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B183" s="2">
+        <v>17</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B184" s="2">
+        <v>18</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B185" s="2">
+        <v>24</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B186" s="2">
+        <v>18</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B187" s="2">
+        <v>18</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D187" s="2"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B188" s="2">
+        <v>21</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D188" s="2"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B189" s="2">
+        <v>19</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B190" s="2">
+        <v>22</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D190" s="2"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B191" s="2">
+        <v>18</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D191" s="2"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B192" s="2">
+        <v>17</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D192" s="2"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B193" s="2">
+        <v>42</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D193" s="2"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B194" s="2">
+        <v>21</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D194" s="2"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B195" s="2">
+        <v>22</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D195" s="2"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B196" s="2">
+        <v>23</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D196" s="2"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B197" s="2">
+        <v>21</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D197" s="2"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B198" s="2">
+        <v>23</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B199" s="2">
+        <v>18</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D199" s="2"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B200" s="2">
+        <v>22</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B201" s="2">
+        <v>18</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D201" s="2"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B202" s="2">
+        <v>18</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D202" s="2"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B203" s="2">
+        <v>19</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D203" s="2"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B204" s="2">
+        <v>30</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D204" s="2"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B205" s="2">
+        <v>24</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D205" s="2"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>155</v>
+      </c>
+      <c r="B206">
+        <v>19</v>
+      </c>
+      <c r="C206" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B207" s="3">
+        <v>26</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B208" s="3">
+        <v>18</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B209" s="3">
+        <v>20</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D209" s="3"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B210" s="3">
+        <v>27</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D210" s="3"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B211" s="3">
+        <v>19</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B212" s="1">
+        <v>26</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D212" s="1"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B213" s="1">
+        <v>26</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D213" s="1"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B214" s="1">
+        <v>21</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D214" s="1"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B215" s="1">
+        <v>21</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D215" s="1"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B216" s="1">
+        <v>47</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D216" s="1"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D227">
+    <sortCondition ref="D2:D227"/>
+    <sortCondition ref="C2:C227"/>
+    <sortCondition ref="A2:A227"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>